<commit_message>
update excel without excel file
</commit_message>
<xml_diff>
--- a/api/PromptStyle.xlsx
+++ b/api/PromptStyle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiaxin\Desktop\SD Web UI\SD-UI\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E05C32-AC90-484F-A0A5-244FD4B8B7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293954A5-12C1-468D-AD71-119FCF82E9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12450" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Style</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">None </t>
   </si>
 </sst>
 </file>
@@ -453,16 +459,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" activeCellId="1" sqref="C13:D15 N16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -479,10 +485,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -490,10 +496,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -501,10 +507,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -512,10 +518,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -523,10 +529,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -534,10 +540,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -545,10 +551,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -556,12 +562,23 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>